<commit_message>
avances en varias partes del documento
</commit_message>
<xml_diff>
--- a/ceia/Book1.xlsx
+++ b/ceia/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricio.denardi/Documents/CEIA/GdP/repos/Plantilla-planificacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricio.denardi/MIA/GdP/repos/MIA_01c_GdP/ceia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F581B0C1-EA71-8B4E-A9C4-0B948CFE4D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5930891D-9912-6B4A-8F07-8809655CFA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{60506E37-6694-4945-AB2D-66CEB6A8BECA}"/>
+    <workbookView xWindow="4080" yWindow="620" windowWidth="30240" windowHeight="17080" xr2:uid="{60506E37-6694-4945-AB2D-66CEB6A8BECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <t>Etapa del desarrollo de la aplicación para celulares.</t>
   </si>
   <si>
-    <t>Defensa del trabajoj final.</t>
+    <t>Defensa del trabajo  final.</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A37993B-F382-E941-A321-BC74B92DAEB5}">
   <dimension ref="E4:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>